<commit_message>
Day36. [LeetCode-#412] Fizz Buzz
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423A6BE7-97D3-4226-9043-E512E166964D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F63C8E-1A24-4189-9024-ABEEFF90D057}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21525" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="124">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,15 +129,6 @@
     <t>Day32</t>
   </si>
   <si>
-    <t>Day33</t>
-  </si>
-  <si>
-    <t>Day34</t>
-  </si>
-  <si>
-    <t>Day35</t>
-  </si>
-  <si>
     <t>Day36</t>
   </si>
   <si>
@@ -325,12 +316,6 @@
   </si>
   <si>
     <t>Day98</t>
-  </si>
-  <si>
-    <t>Day99</t>
-  </si>
-  <si>
-    <t>Day100</t>
   </si>
   <si>
     <t>類型</t>
@@ -369,15 +354,6 @@
   </si>
   <si>
     <t>LeetCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nested for loop, If statement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Iterate through Nested for loop
-2. if nums[i]==nums[j]  &amp;&amp;  i &lt; j, Good pairs add 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -407,14 +383,6 @@
       </rPr>
       <t>x1,y1,x2,y2,...,xn,yn]</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create new Array, Check Even or Odd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LINQ,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -489,6 +457,101 @@
       </rPr>
       <t>that the richest customer has</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a custome Login page in ASP.NET Core MVC </t>
+  </si>
+  <si>
+    <t>1. Create a ASP.NET Core MVC Project
+2. Add New Scaffolded Identity
+    1. Select existing layout 
+    &gt; Views\Shared\_Layout.cshtml
+    2. Choose file to override
+    &gt; Account\Login, 
+    &gt; Account\Register
+    3. Add Data Context:
+    &gt; Auth.System.Data.AuthDbContext
+    4. Add User Class
+    &gt; ApplicationUser
+  * Change font-family
+  * Change layout
+  * Add profile data for application users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Update Startup.cs
+  &gt; services.addRazorPages();
+  &gt; app.UseAuthentication();
+  &gt; endpoints.MapRazorPages();
+4. Change font
+5. Add connection string
+  &gt;appsettings.json
+6. Add-Migration
+  &gt; Add-Migration "Initial-Create"
+  &gt; Update-Database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>依據條件產生新的 Array</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Iterate through Nested </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or loop
+2. if nums[i]==nums[j]  &amp;&amp;  i &lt; j, Good pairs add 1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* LINQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Create new Array
+* Check Even or Odd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Nested For loop, 
+* If statement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Array.Clone()
+* While loop  less than
+* If statement</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -571,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,6 +656,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1034,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1045,8 +1111,8 @@
     <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1055,25 +1121,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15">
@@ -1084,14 +1150,14 @@
         <v>44154</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
@@ -1102,14 +1168,14 @@
         <v>44155</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15">
@@ -1120,14 +1186,14 @@
         <v>44156</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
@@ -1138,14 +1204,14 @@
         <v>44157</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
@@ -1156,14 +1222,14 @@
         <v>44158</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
@@ -1174,14 +1240,14 @@
         <v>44159</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15">
@@ -1192,14 +1258,14 @@
         <v>44160</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15">
@@ -1210,14 +1276,14 @@
         <v>44161</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15">
@@ -1228,14 +1294,14 @@
         <v>44162</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15">
@@ -1246,14 +1312,14 @@
         <v>44163</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15">
@@ -1264,14 +1330,14 @@
         <v>44164</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15">
@@ -1282,14 +1348,14 @@
         <v>44165</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15">
@@ -1300,14 +1366,14 @@
         <v>44166</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15">
@@ -1318,14 +1384,14 @@
         <v>44167</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15">
@@ -1336,14 +1402,14 @@
         <v>44168</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15">
@@ -1354,14 +1420,14 @@
         <v>44169</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15">
@@ -1372,14 +1438,14 @@
         <v>44170</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15">
@@ -1390,14 +1456,14 @@
         <v>44171</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15">
@@ -1408,14 +1474,14 @@
         <v>44172</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15">
@@ -1426,14 +1492,14 @@
         <v>44173</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15">
@@ -1444,14 +1510,14 @@
         <v>44174</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15">
@@ -1462,14 +1528,14 @@
         <v>44175</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15">
@@ -1480,14 +1546,14 @@
         <v>44176</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15">
@@ -1498,14 +1564,14 @@
         <v>44177</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15">
@@ -1516,14 +1582,14 @@
         <v>44178</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15">
@@ -1534,14 +1600,14 @@
         <v>44179</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15">
@@ -1552,14 +1618,14 @@
         <v>44180</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15">
@@ -1570,17 +1636,19 @@
         <v>44181</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
@@ -1588,14 +1656,20 @@
         <v>44182</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="H30" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="16.5">
@@ -1606,23 +1680,23 @@
         <v>44183</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E31" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15">
+      <c r="H31" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
@@ -1630,23 +1704,23 @@
         <v>44184</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>117</v>
+      <c r="F32" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="71.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="43.5">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -1654,73 +1728,91 @@
         <v>44185</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>110</v>
+      <c r="F33" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="99.75">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="57">
       <c r="A34" s="5" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="B34" s="6">
         <v>44186</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" hidden="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="261" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="B35" s="6">
+        <v>44187</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" hidden="1">
+      <c r="G35" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="185.25">
       <c r="A36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="B36" s="6">
+        <v>44188</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" hidden="1">
+      <c r="G36" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H36" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="5"/>
@@ -1730,9 +1822,9 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" ht="15" hidden="1">
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="5"/>
@@ -1742,9 +1834,9 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" ht="15" hidden="1">
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="5"/>
@@ -1754,9 +1846,9 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="1:8" ht="15" hidden="1">
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="5"/>
@@ -1766,9 +1858,9 @@
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="1:8" ht="15" hidden="1">
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
@@ -1778,9 +1870,9 @@
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="1:8" ht="15" hidden="1">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
@@ -1790,9 +1882,9 @@
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="1:8" ht="15" hidden="1">
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="5"/>
@@ -1802,9 +1894,9 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="1:8" ht="15" hidden="1">
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="5"/>
@@ -1814,9 +1906,9 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="1:8" ht="15" hidden="1">
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="5"/>
@@ -1826,9 +1918,9 @@
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="1:8" ht="15" hidden="1">
+    <row r="46" spans="1:8" ht="15">
       <c r="A46" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="5"/>
@@ -1838,9 +1930,9 @@
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" spans="1:8" ht="15" hidden="1">
+    <row r="47" spans="1:8" ht="15">
       <c r="A47" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="5"/>
@@ -1850,9 +1942,9 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="1:8" ht="15" hidden="1">
+    <row r="48" spans="1:8" ht="15">
       <c r="A48" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
@@ -1862,9 +1954,9 @@
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="1:8" ht="15" hidden="1">
+    <row r="49" spans="1:8" ht="15">
       <c r="A49" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="5"/>
@@ -1874,9 +1966,9 @@
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" spans="1:8" ht="15" hidden="1">
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="5"/>
@@ -1886,9 +1978,9 @@
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" spans="1:8" ht="15" hidden="1">
+    <row r="51" spans="1:8" ht="15">
       <c r="A51" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="5"/>
@@ -1898,9 +1990,9 @@
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="1:8" ht="15" hidden="1">
+    <row r="52" spans="1:8" ht="15">
       <c r="A52" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="5"/>
@@ -1910,9 +2002,9 @@
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="1:8" ht="15" hidden="1">
+    <row r="53" spans="1:8" ht="15">
       <c r="A53" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="5"/>
@@ -1922,9 +2014,9 @@
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="1:8" ht="15" hidden="1">
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="5"/>
@@ -1934,9 +2026,9 @@
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="55" spans="1:8" ht="15" hidden="1">
+    <row r="55" spans="1:8" ht="15">
       <c r="A55" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="5"/>
@@ -1946,9 +2038,9 @@
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
     </row>
-    <row r="56" spans="1:8" ht="15" hidden="1">
+    <row r="56" spans="1:8" ht="15">
       <c r="A56" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="5"/>
@@ -1958,9 +2050,9 @@
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="1:8" ht="15" hidden="1">
+    <row r="57" spans="1:8" ht="15">
       <c r="A57" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="5"/>
@@ -1970,9 +2062,9 @@
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="1:8" ht="15" hidden="1">
+    <row r="58" spans="1:8" ht="15">
       <c r="A58" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="5"/>
@@ -1982,9 +2074,9 @@
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
     </row>
-    <row r="59" spans="1:8" ht="15" hidden="1">
+    <row r="59" spans="1:8" ht="15">
       <c r="A59" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="5"/>
@@ -1994,9 +2086,9 @@
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="1:8" ht="15" hidden="1">
+    <row r="60" spans="1:8" ht="15">
       <c r="A60" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="5"/>
@@ -2006,9 +2098,9 @@
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
     </row>
-    <row r="61" spans="1:8" ht="15" hidden="1">
+    <row r="61" spans="1:8" ht="15">
       <c r="A61" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="5"/>
@@ -2018,9 +2110,9 @@
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
     </row>
-    <row r="62" spans="1:8" ht="15" hidden="1">
+    <row r="62" spans="1:8" ht="15">
       <c r="A62" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="5"/>
@@ -2030,9 +2122,9 @@
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="1:8" ht="15" hidden="1">
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="5"/>
@@ -2042,9 +2134,9 @@
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
     </row>
-    <row r="64" spans="1:8" ht="15" hidden="1">
+    <row r="64" spans="1:8" ht="15">
       <c r="A64" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="5"/>
@@ -2054,9 +2146,9 @@
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
     </row>
-    <row r="65" spans="1:8" ht="15" hidden="1">
+    <row r="65" spans="1:8" ht="15">
       <c r="A65" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="5"/>
@@ -2066,9 +2158,9 @@
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66" spans="1:8" ht="15" hidden="1">
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="5"/>
@@ -2078,9 +2170,9 @@
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
     </row>
-    <row r="67" spans="1:8" ht="15" hidden="1">
+    <row r="67" spans="1:8" ht="15">
       <c r="A67" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="5"/>
@@ -2090,9 +2182,9 @@
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
     </row>
-    <row r="68" spans="1:8" ht="15" hidden="1">
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="5"/>
@@ -2102,9 +2194,9 @@
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
-    <row r="69" spans="1:8" ht="15" hidden="1">
+    <row r="69" spans="1:8" ht="15">
       <c r="A69" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="5"/>
@@ -2114,9 +2206,9 @@
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
     </row>
-    <row r="70" spans="1:8" ht="15" hidden="1">
+    <row r="70" spans="1:8" ht="15">
       <c r="A70" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="5"/>
@@ -2126,9 +2218,9 @@
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
     </row>
-    <row r="71" spans="1:8" ht="15" hidden="1">
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="5"/>
@@ -2138,9 +2230,9 @@
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
     </row>
-    <row r="72" spans="1:8" ht="15" hidden="1">
+    <row r="72" spans="1:8" ht="15">
       <c r="A72" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="5"/>
@@ -2150,9 +2242,9 @@
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
     </row>
-    <row r="73" spans="1:8" ht="15" hidden="1">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="5"/>
@@ -2162,9 +2254,9 @@
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
     </row>
-    <row r="74" spans="1:8" ht="15" hidden="1">
+    <row r="74" spans="1:8" ht="15">
       <c r="A74" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="5"/>
@@ -2174,9 +2266,9 @@
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
     </row>
-    <row r="75" spans="1:8" ht="15" hidden="1">
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="5"/>
@@ -2186,9 +2278,9 @@
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
     </row>
-    <row r="76" spans="1:8" ht="15" hidden="1">
+    <row r="76" spans="1:8" ht="15">
       <c r="A76" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="5"/>
@@ -2198,9 +2290,9 @@
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
     </row>
-    <row r="77" spans="1:8" ht="15" hidden="1">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="5"/>
@@ -2210,9 +2302,9 @@
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
     </row>
-    <row r="78" spans="1:8" ht="15" hidden="1">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="5"/>
@@ -2222,9 +2314,9 @@
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
     </row>
-    <row r="79" spans="1:8" ht="15" hidden="1">
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="5"/>
@@ -2234,9 +2326,9 @@
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
     </row>
-    <row r="80" spans="1:8" ht="15" hidden="1">
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="5"/>
@@ -2246,9 +2338,9 @@
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
     </row>
-    <row r="81" spans="1:8" ht="15" hidden="1">
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="5"/>
@@ -2258,9 +2350,9 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
     </row>
-    <row r="82" spans="1:8" ht="15" hidden="1">
+    <row r="82" spans="1:8" ht="15">
       <c r="A82" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="5"/>
@@ -2270,9 +2362,9 @@
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
     </row>
-    <row r="83" spans="1:8" ht="15" hidden="1">
+    <row r="83" spans="1:8" ht="15">
       <c r="A83" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B83" s="6"/>
       <c r="C83" s="5"/>
@@ -2282,9 +2374,9 @@
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
     </row>
-    <row r="84" spans="1:8" ht="15" hidden="1">
+    <row r="84" spans="1:8" ht="15">
       <c r="A84" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B84" s="6"/>
       <c r="C84" s="5"/>
@@ -2294,9 +2386,9 @@
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
     </row>
-    <row r="85" spans="1:8" ht="15" hidden="1">
+    <row r="85" spans="1:8" ht="15">
       <c r="A85" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B85" s="6"/>
       <c r="C85" s="5"/>
@@ -2306,9 +2398,9 @@
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
     </row>
-    <row r="86" spans="1:8" ht="15" hidden="1">
+    <row r="86" spans="1:8" ht="15">
       <c r="A86" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="5"/>
@@ -2318,9 +2410,9 @@
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
     </row>
-    <row r="87" spans="1:8" ht="15" hidden="1">
+    <row r="87" spans="1:8" ht="15">
       <c r="A87" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87" s="5"/>
@@ -2330,9 +2422,9 @@
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
     </row>
-    <row r="88" spans="1:8" ht="15" hidden="1">
+    <row r="88" spans="1:8" ht="15">
       <c r="A88" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="5"/>
@@ -2342,9 +2434,9 @@
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
     </row>
-    <row r="89" spans="1:8" ht="15" hidden="1">
+    <row r="89" spans="1:8" ht="15">
       <c r="A89" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="5"/>
@@ -2354,9 +2446,9 @@
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
     </row>
-    <row r="90" spans="1:8" ht="15" hidden="1">
+    <row r="90" spans="1:8" ht="15">
       <c r="A90" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="5"/>
@@ -2366,9 +2458,9 @@
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
     </row>
-    <row r="91" spans="1:8" ht="15" hidden="1">
+    <row r="91" spans="1:8" ht="15">
       <c r="A91" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="5"/>
@@ -2378,9 +2470,9 @@
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
     </row>
-    <row r="92" spans="1:8" ht="15" hidden="1">
+    <row r="92" spans="1:8" ht="15">
       <c r="A92" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="5"/>
@@ -2390,9 +2482,9 @@
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
     </row>
-    <row r="93" spans="1:8" ht="15" hidden="1">
+    <row r="93" spans="1:8" ht="15">
       <c r="A93" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="5"/>
@@ -2402,9 +2494,9 @@
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
     </row>
-    <row r="94" spans="1:8" ht="15" hidden="1">
+    <row r="94" spans="1:8" ht="15">
       <c r="A94" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B94" s="6"/>
       <c r="C94" s="5"/>
@@ -2414,9 +2506,9 @@
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
     </row>
-    <row r="95" spans="1:8" ht="15" hidden="1">
+    <row r="95" spans="1:8" ht="15">
       <c r="A95" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B95" s="6"/>
       <c r="C95" s="5"/>
@@ -2426,9 +2518,9 @@
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
     </row>
-    <row r="96" spans="1:8" ht="15" hidden="1">
+    <row r="96" spans="1:8" ht="15">
       <c r="A96" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B96" s="6"/>
       <c r="C96" s="5"/>
@@ -2438,9 +2530,9 @@
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
     </row>
-    <row r="97" spans="1:8" ht="15" hidden="1">
+    <row r="97" spans="1:8" ht="15">
       <c r="A97" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B97" s="6"/>
       <c r="C97" s="5"/>
@@ -2450,9 +2542,9 @@
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
     </row>
-    <row r="98" spans="1:8" ht="15" hidden="1">
+    <row r="98" spans="1:8" ht="15">
       <c r="A98" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B98" s="6"/>
       <c r="C98" s="5"/>
@@ -2462,9 +2554,9 @@
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
     </row>
-    <row r="99" spans="1:8" ht="15" hidden="1">
+    <row r="99" spans="1:8" ht="15">
       <c r="A99" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B99" s="6"/>
       <c r="C99" s="5"/>
@@ -2474,10 +2566,8 @@
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
     </row>
-    <row r="100" spans="1:8" ht="15" hidden="1">
-      <c r="A100" s="5" t="s">
-        <v>99</v>
-      </c>
+    <row r="100" spans="1:8" ht="267.75" customHeight="1">
+      <c r="A100" s="5"/>
       <c r="B100" s="6"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -2486,10 +2576,8 @@
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
     </row>
-    <row r="101" spans="1:8" ht="15" hidden="1">
-      <c r="A101" s="5" t="s">
-        <v>100</v>
-      </c>
+    <row r="101" spans="1:8" ht="15">
+      <c r="A101" s="5"/>
       <c r="B101" s="6"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>

</xml_diff>

<commit_message>
Day37 [LeetCode-#415] Add Strings
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9807323-0589-4B7C-9DB6-27ED9B4F79E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6132918B-7BCF-44AA-AD0D-157884122BAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="129">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -568,6 +568,12 @@
 4. if for multiples of five, output Buzz,
 5. if for multiples of three and multiples of five, output FizzBuzz</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day99</t>
+  </si>
+  <si>
+    <t>Day100</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1116,10 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2590,8 +2596,10 @@
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
     </row>
-    <row r="100" spans="1:8" ht="267.75" customHeight="1">
-      <c r="A100" s="5"/>
+    <row r="100" spans="1:8" ht="15">
+      <c r="A100" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="B100" s="6"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -2601,14 +2609,9 @@
       <c r="H100" s="7"/>
     </row>
     <row r="101" spans="1:8" ht="15">
-      <c r="A101" s="5"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="7"/>
-      <c r="G101" s="7"/>
-      <c r="H101" s="7"/>
+      <c r="A101" s="5" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Day38 [LeetCode-#20] Valid Parentheses
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1856E09-377A-4643-8430-A56060CC7D9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A25920-C387-4394-BDF9-3BD42E74665F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="132">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -575,6 +575,17 @@
   <si>
     <t>Day100</t>
   </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Return the sum of num1 and num2</t>
+  </si>
+  <si>
+    <t>Program to determine if the input string is valid or not</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -583,7 +594,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,6 +645,12 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF263238"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -655,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -682,6 +699,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1115,11 +1133,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1856,22 +1874,38 @@
       <c r="A38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="B38" s="6">
+        <v>44190</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8" ht="16.5">
       <c r="A39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="B39" s="6">
+        <v>44191</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>

</xml_diff>

<commit_message>
Day39 [LeetCode-155] Min Stack
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A25920-C387-4394-BDF9-3BD42E74665F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF41D80-9FEE-429D-ADC7-CF0814FA68CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
+    <sheet name="Skill" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="135">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -323,10 +333,6 @@
   </si>
   <si>
     <t>日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>所花費時間</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -586,13 +592,42 @@
     <t>Program to determine if the input string is valid or not</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>所花費時間</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>(hr)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design a stack that supports push, pop, top, and retrieving the minimum element in constant time.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -672,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -700,13 +735,46 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -852,17 +920,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{810993BB-277E-4BBC-8D8A-6CC291D7C060}" name="表格1" displayName="表格1" ref="A1:H101" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{810993BB-277E-4BBC-8D8A-6CC291D7C060}" name="表格1" displayName="表格1" ref="A1:H101" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:H101" xr:uid="{9C8C2E40-E16F-435F-9A43-053065E55DB4}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{99B64B0C-7B02-42F0-9370-CE94A9D8F63E}" name="天數" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{6DB2B110-1A72-42DF-A8B1-B343A1A0C427}" name="日期" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E2F17329-26C5-4449-AAAF-C99CB7FEDC95}" name="類型" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{C61EBE76-371E-4E92-9EC6-7A0DCD08BB8F}" name="Topic" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{31DC304D-1D42-4DAF-B0CC-BDF494F91A9F}" name="Purpose" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{8148EAA2-148F-4A8C-92EC-EB9EE7D7668D}" name="Skill" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{04FB5744-EEEA-494D-902D-6F2FC2E61962}" name="Step by Step" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{F9A548FB-04A0-4F7C-AEDA-6DA3F2B4B3EE}" name="所花費時間" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{99B64B0C-7B02-42F0-9370-CE94A9D8F63E}" name="天數" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{6DB2B110-1A72-42DF-A8B1-B343A1A0C427}" name="日期" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{E2F17329-26C5-4449-AAAF-C99CB7FEDC95}" name="類型" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{C61EBE76-371E-4E92-9EC6-7A0DCD08BB8F}" name="Topic" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{31DC304D-1D42-4DAF-B0CC-BDF494F91A9F}" name="Purpose" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8148EAA2-148F-4A8C-92EC-EB9EE7D7668D}" name="Skill" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{04FB5744-EEEA-494D-902D-6F2FC2E61962}" name="Step by Step" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F9A548FB-04A0-4F7C-AEDA-6DA3F2B4B3EE}" name="所花費時間(hr)" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AABD3024-27F9-4340-9F92-F8142ABB2B4D}" name="表格2" displayName="表格2" ref="A1:B2" insertRow="1" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B2" xr:uid="{319BFF1A-00BE-462B-A13D-51F0FB7E00A8}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3C41B99C-6466-4DFC-B371-702A032EAC39}" name="Skill" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{EF89176C-D56C-42F7-B7FE-8446C1093E92}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1131,13 +1210,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomRight" activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1146,10 +1225,11 @@
     <col min="2" max="2" width="12.5" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="90.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15">
@@ -1163,19 +1243,19 @@
         <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15">
@@ -1186,14 +1266,14 @@
         <v>44154</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
@@ -1204,14 +1284,14 @@
         <v>44155</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15">
@@ -1222,14 +1302,14 @@
         <v>44156</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
@@ -1240,14 +1320,14 @@
         <v>44157</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
@@ -1258,14 +1338,14 @@
         <v>44158</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
@@ -1276,14 +1356,14 @@
         <v>44159</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15">
@@ -1294,14 +1374,14 @@
         <v>44160</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15">
@@ -1312,14 +1392,14 @@
         <v>44161</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15">
@@ -1330,14 +1410,14 @@
         <v>44162</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15">
@@ -1348,14 +1428,14 @@
         <v>44163</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15">
@@ -1366,14 +1446,14 @@
         <v>44164</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15">
@@ -1384,14 +1464,14 @@
         <v>44165</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15">
@@ -1402,14 +1482,14 @@
         <v>44166</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15">
@@ -1420,14 +1500,14 @@
         <v>44167</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15">
@@ -1438,14 +1518,14 @@
         <v>44168</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15">
@@ -1456,14 +1536,14 @@
         <v>44169</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15">
@@ -1474,14 +1554,14 @@
         <v>44170</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15">
@@ -1492,14 +1572,14 @@
         <v>44171</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15">
@@ -1510,14 +1590,14 @@
         <v>44172</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15">
@@ -1528,14 +1608,14 @@
         <v>44173</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15">
@@ -1546,14 +1626,14 @@
         <v>44174</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15">
@@ -1564,14 +1644,14 @@
         <v>44175</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15">
@@ -1582,14 +1662,14 @@
         <v>44176</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15">
@@ -1600,14 +1680,14 @@
         <v>44177</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15">
@@ -1618,14 +1698,14 @@
         <v>44178</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15">
@@ -1636,14 +1716,14 @@
         <v>44179</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15">
@@ -1654,14 +1734,14 @@
         <v>44180</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15">
@@ -1672,16 +1752,16 @@
         <v>44181</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="45">
@@ -1692,20 +1772,20 @@
         <v>44182</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="16.5">
@@ -1716,20 +1796,20 @@
         <v>44183</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="1">
-        <v>60</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30">
@@ -1740,23 +1820,23 @@
         <v>44184</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="43.5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="43.5">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -1764,89 +1844,88 @@
         <v>44185</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="57">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="57">
       <c r="A34" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" s="6">
         <v>44186</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="261" customHeight="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="261" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="6">
         <v>44187</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" ht="185.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="185.25">
       <c r="A36" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="6">
         <v>44188</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H36" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="85.5">
+    <row r="37" spans="1:11" ht="85.5">
       <c r="A37" s="5" t="s">
         <v>33</v>
       </c>
@@ -1854,23 +1933,23 @@
         <v>44189</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="H37" s="7">
+        <v>125</v>
+      </c>
+      <c r="H37" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:11" ht="15">
       <c r="A38" s="5" t="s">
         <v>34</v>
       </c>
@@ -1878,19 +1957,18 @@
         <v>44190</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:8" ht="16.5">
+    </row>
+    <row r="39" spans="1:11" ht="16.5">
       <c r="A39" s="5" t="s">
         <v>35</v>
       </c>
@@ -1898,31 +1976,44 @@
         <v>44191</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" ht="15">
+      <c r="H39" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="16.5">
       <c r="A40" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+      <c r="B40" s="6">
+        <v>44192</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>134</v>
+      </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8" ht="15">
+      <c r="H40" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="K40" s="12"/>
+    </row>
+    <row r="41" spans="1:11" ht="15">
       <c r="A41" s="5" t="s">
         <v>37</v>
       </c>
@@ -1932,9 +2023,8 @@
       <c r="E41" s="5"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="1:8" ht="15">
+    </row>
+    <row r="42" spans="1:11" ht="15">
       <c r="A42" s="5" t="s">
         <v>38</v>
       </c>
@@ -1944,9 +2034,8 @@
       <c r="E42" s="5"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-    </row>
-    <row r="43" spans="1:8" ht="15">
+    </row>
+    <row r="43" spans="1:11" ht="15">
       <c r="A43" s="5" t="s">
         <v>39</v>
       </c>
@@ -1956,9 +2045,8 @@
       <c r="E43" s="5"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:8" ht="15">
+    </row>
+    <row r="44" spans="1:11" ht="15">
       <c r="A44" s="5" t="s">
         <v>40</v>
       </c>
@@ -1968,9 +2056,8 @@
       <c r="E44" s="5"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:8" ht="15">
+    </row>
+    <row r="45" spans="1:11" ht="15">
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
@@ -1980,9 +2067,8 @@
       <c r="E45" s="5"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:8" ht="15">
+    </row>
+    <row r="46" spans="1:11" ht="15">
       <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
@@ -1992,9 +2078,8 @@
       <c r="E46" s="5"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" ht="15">
+    </row>
+    <row r="47" spans="1:11" ht="15">
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
@@ -2004,9 +2089,8 @@
       <c r="E47" s="5"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="1:8" ht="15">
+    </row>
+    <row r="48" spans="1:11" ht="15">
       <c r="A48" s="5" t="s">
         <v>44</v>
       </c>
@@ -2016,9 +2100,8 @@
       <c r="E48" s="5"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:8" ht="15">
+    </row>
+    <row r="49" spans="1:7" ht="15">
       <c r="A49" s="5" t="s">
         <v>45</v>
       </c>
@@ -2028,9 +2111,8 @@
       <c r="E49" s="5"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="1:8" ht="15">
+    </row>
+    <row r="50" spans="1:7" ht="15">
       <c r="A50" s="5" t="s">
         <v>46</v>
       </c>
@@ -2040,9 +2122,8 @@
       <c r="E50" s="5"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="1:8" ht="15">
+    </row>
+    <row r="51" spans="1:7" ht="15">
       <c r="A51" s="5" t="s">
         <v>47</v>
       </c>
@@ -2052,9 +2133,8 @@
       <c r="E51" s="5"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-    </row>
-    <row r="52" spans="1:8" ht="15">
+    </row>
+    <row r="52" spans="1:7" ht="15">
       <c r="A52" s="5" t="s">
         <v>48</v>
       </c>
@@ -2064,9 +2144,8 @@
       <c r="E52" s="5"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:8" ht="15">
+    </row>
+    <row r="53" spans="1:7" ht="15">
       <c r="A53" s="5" t="s">
         <v>49</v>
       </c>
@@ -2076,9 +2155,8 @@
       <c r="E53" s="5"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="1:8" ht="15">
+    </row>
+    <row r="54" spans="1:7" ht="15">
       <c r="A54" s="5" t="s">
         <v>50</v>
       </c>
@@ -2088,9 +2166,8 @@
       <c r="E54" s="5"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:8" ht="15">
+    </row>
+    <row r="55" spans="1:7" ht="15">
       <c r="A55" s="5" t="s">
         <v>51</v>
       </c>
@@ -2100,9 +2177,8 @@
       <c r="E55" s="5"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:8" ht="15">
+    </row>
+    <row r="56" spans="1:7" ht="15">
       <c r="A56" s="5" t="s">
         <v>52</v>
       </c>
@@ -2112,9 +2188,8 @@
       <c r="E56" s="5"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-    </row>
-    <row r="57" spans="1:8" ht="15">
+    </row>
+    <row r="57" spans="1:7" ht="15">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
@@ -2124,9 +2199,8 @@
       <c r="E57" s="5"/>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-    </row>
-    <row r="58" spans="1:8" ht="15">
+    </row>
+    <row r="58" spans="1:7" ht="15">
       <c r="A58" s="5" t="s">
         <v>54</v>
       </c>
@@ -2136,9 +2210,8 @@
       <c r="E58" s="5"/>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="1:8" ht="15">
+    </row>
+    <row r="59" spans="1:7" ht="15">
       <c r="A59" s="5" t="s">
         <v>55</v>
       </c>
@@ -2148,9 +2221,8 @@
       <c r="E59" s="5"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:8" ht="15">
+    </row>
+    <row r="60" spans="1:7" ht="15">
       <c r="A60" s="5" t="s">
         <v>56</v>
       </c>
@@ -2160,9 +2232,8 @@
       <c r="E60" s="5"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:8" ht="15">
+    </row>
+    <row r="61" spans="1:7" ht="15">
       <c r="A61" s="5" t="s">
         <v>57</v>
       </c>
@@ -2172,9 +2243,8 @@
       <c r="E61" s="5"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:8" ht="15">
+    </row>
+    <row r="62" spans="1:7" ht="15">
       <c r="A62" s="5" t="s">
         <v>58</v>
       </c>
@@ -2184,9 +2254,8 @@
       <c r="E62" s="5"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:8" ht="15">
+    </row>
+    <row r="63" spans="1:7" ht="15">
       <c r="A63" s="5" t="s">
         <v>59</v>
       </c>
@@ -2196,9 +2265,8 @@
       <c r="E63" s="5"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:8" ht="15">
+    </row>
+    <row r="64" spans="1:7" ht="15">
       <c r="A64" s="5" t="s">
         <v>60</v>
       </c>
@@ -2208,9 +2276,8 @@
       <c r="E64" s="5"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="1:8" ht="15">
+    </row>
+    <row r="65" spans="1:7" ht="15">
       <c r="A65" s="5" t="s">
         <v>61</v>
       </c>
@@ -2220,9 +2287,8 @@
       <c r="E65" s="5"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-    </row>
-    <row r="66" spans="1:8" ht="15">
+    </row>
+    <row r="66" spans="1:7" ht="15">
       <c r="A66" s="5" t="s">
         <v>62</v>
       </c>
@@ -2232,9 +2298,8 @@
       <c r="E66" s="5"/>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:8" ht="15">
+    </row>
+    <row r="67" spans="1:7" ht="15">
       <c r="A67" s="5" t="s">
         <v>63</v>
       </c>
@@ -2244,9 +2309,8 @@
       <c r="E67" s="5"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-    </row>
-    <row r="68" spans="1:8" ht="15">
+    </row>
+    <row r="68" spans="1:7" ht="15">
       <c r="A68" s="5" t="s">
         <v>64</v>
       </c>
@@ -2256,9 +2320,8 @@
       <c r="E68" s="5"/>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="1:8" ht="15">
+    </row>
+    <row r="69" spans="1:7" ht="15">
       <c r="A69" s="5" t="s">
         <v>65</v>
       </c>
@@ -2268,9 +2331,8 @@
       <c r="E69" s="5"/>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="1:8" ht="15">
+    </row>
+    <row r="70" spans="1:7" ht="15">
       <c r="A70" s="5" t="s">
         <v>66</v>
       </c>
@@ -2280,9 +2342,8 @@
       <c r="E70" s="5"/>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-    </row>
-    <row r="71" spans="1:8" ht="15">
+    </row>
+    <row r="71" spans="1:7" ht="15">
       <c r="A71" s="5" t="s">
         <v>67</v>
       </c>
@@ -2292,9 +2353,8 @@
       <c r="E71" s="5"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-    </row>
-    <row r="72" spans="1:8" ht="15">
+    </row>
+    <row r="72" spans="1:7" ht="15">
       <c r="A72" s="5" t="s">
         <v>68</v>
       </c>
@@ -2304,9 +2364,8 @@
       <c r="E72" s="5"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-    </row>
-    <row r="73" spans="1:8" ht="15">
+    </row>
+    <row r="73" spans="1:7" ht="15">
       <c r="A73" s="5" t="s">
         <v>69</v>
       </c>
@@ -2316,9 +2375,8 @@
       <c r="E73" s="5"/>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-    </row>
-    <row r="74" spans="1:8" ht="15">
+    </row>
+    <row r="74" spans="1:7" ht="15">
       <c r="A74" s="5" t="s">
         <v>70</v>
       </c>
@@ -2328,9 +2386,8 @@
       <c r="E74" s="5"/>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-    </row>
-    <row r="75" spans="1:8" ht="15">
+    </row>
+    <row r="75" spans="1:7" ht="15">
       <c r="A75" s="5" t="s">
         <v>71</v>
       </c>
@@ -2340,9 +2397,8 @@
       <c r="E75" s="5"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-    </row>
-    <row r="76" spans="1:8" ht="15">
+    </row>
+    <row r="76" spans="1:7" ht="15">
       <c r="A76" s="5" t="s">
         <v>72</v>
       </c>
@@ -2352,9 +2408,8 @@
       <c r="E76" s="5"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
-    </row>
-    <row r="77" spans="1:8" ht="15">
+    </row>
+    <row r="77" spans="1:7" ht="15">
       <c r="A77" s="5" t="s">
         <v>73</v>
       </c>
@@ -2364,9 +2419,8 @@
       <c r="E77" s="5"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
-    </row>
-    <row r="78" spans="1:8" ht="15">
+    </row>
+    <row r="78" spans="1:7" ht="15">
       <c r="A78" s="5" t="s">
         <v>74</v>
       </c>
@@ -2376,9 +2430,8 @@
       <c r="E78" s="5"/>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-    </row>
-    <row r="79" spans="1:8" ht="15">
+    </row>
+    <row r="79" spans="1:7" ht="15">
       <c r="A79" s="5" t="s">
         <v>75</v>
       </c>
@@ -2388,9 +2441,8 @@
       <c r="E79" s="5"/>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-    </row>
-    <row r="80" spans="1:8" ht="15">
+    </row>
+    <row r="80" spans="1:7" ht="15">
       <c r="A80" s="5" t="s">
         <v>76</v>
       </c>
@@ -2400,9 +2452,8 @@
       <c r="E80" s="5"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
-    </row>
-    <row r="81" spans="1:8" ht="15">
+    </row>
+    <row r="81" spans="1:7" ht="15">
       <c r="A81" s="5" t="s">
         <v>77</v>
       </c>
@@ -2412,9 +2463,8 @@
       <c r="E81" s="5"/>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
-    </row>
-    <row r="82" spans="1:8" ht="15">
+    </row>
+    <row r="82" spans="1:7" ht="15">
       <c r="A82" s="5" t="s">
         <v>78</v>
       </c>
@@ -2424,9 +2474,8 @@
       <c r="E82" s="5"/>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
-      <c r="H82" s="7"/>
-    </row>
-    <row r="83" spans="1:8" ht="15">
+    </row>
+    <row r="83" spans="1:7" ht="15">
       <c r="A83" s="5" t="s">
         <v>79</v>
       </c>
@@ -2436,9 +2485,8 @@
       <c r="E83" s="5"/>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
-    </row>
-    <row r="84" spans="1:8" ht="15">
+    </row>
+    <row r="84" spans="1:7" ht="15">
       <c r="A84" s="5" t="s">
         <v>80</v>
       </c>
@@ -2448,9 +2496,8 @@
       <c r="E84" s="5"/>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
-    </row>
-    <row r="85" spans="1:8" ht="15">
+    </row>
+    <row r="85" spans="1:7" ht="15">
       <c r="A85" s="5" t="s">
         <v>81</v>
       </c>
@@ -2460,9 +2507,8 @@
       <c r="E85" s="5"/>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
-    </row>
-    <row r="86" spans="1:8" ht="15">
+    </row>
+    <row r="86" spans="1:7" ht="15">
       <c r="A86" s="5" t="s">
         <v>82</v>
       </c>
@@ -2472,9 +2518,8 @@
       <c r="E86" s="5"/>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:8" ht="15">
+    </row>
+    <row r="87" spans="1:7" ht="15">
       <c r="A87" s="5" t="s">
         <v>83</v>
       </c>
@@ -2484,9 +2529,8 @@
       <c r="E87" s="5"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
-    </row>
-    <row r="88" spans="1:8" ht="15">
+    </row>
+    <row r="88" spans="1:7" ht="15">
       <c r="A88" s="5" t="s">
         <v>84</v>
       </c>
@@ -2496,9 +2540,8 @@
       <c r="E88" s="5"/>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
-      <c r="H88" s="7"/>
-    </row>
-    <row r="89" spans="1:8" ht="15">
+    </row>
+    <row r="89" spans="1:7" ht="15">
       <c r="A89" s="5" t="s">
         <v>85</v>
       </c>
@@ -2508,9 +2551,8 @@
       <c r="E89" s="5"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-    </row>
-    <row r="90" spans="1:8" ht="15">
+    </row>
+    <row r="90" spans="1:7" ht="15">
       <c r="A90" s="5" t="s">
         <v>86</v>
       </c>
@@ -2520,9 +2562,8 @@
       <c r="E90" s="5"/>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
-      <c r="H90" s="7"/>
-    </row>
-    <row r="91" spans="1:8" ht="15">
+    </row>
+    <row r="91" spans="1:7" ht="15">
       <c r="A91" s="5" t="s">
         <v>87</v>
       </c>
@@ -2532,9 +2573,8 @@
       <c r="E91" s="5"/>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
-    </row>
-    <row r="92" spans="1:8" ht="15">
+    </row>
+    <row r="92" spans="1:7" ht="15">
       <c r="A92" s="5" t="s">
         <v>88</v>
       </c>
@@ -2544,9 +2584,8 @@
       <c r="E92" s="5"/>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
-      <c r="H92" s="7"/>
-    </row>
-    <row r="93" spans="1:8" ht="15">
+    </row>
+    <row r="93" spans="1:7" ht="15">
       <c r="A93" s="5" t="s">
         <v>89</v>
       </c>
@@ -2556,9 +2595,8 @@
       <c r="E93" s="5"/>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-    </row>
-    <row r="94" spans="1:8" ht="15">
+    </row>
+    <row r="94" spans="1:7" ht="15">
       <c r="A94" s="5" t="s">
         <v>90</v>
       </c>
@@ -2568,9 +2606,8 @@
       <c r="E94" s="5"/>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-    </row>
-    <row r="95" spans="1:8" ht="15">
+    </row>
+    <row r="95" spans="1:7" ht="15">
       <c r="A95" s="5" t="s">
         <v>91</v>
       </c>
@@ -2580,9 +2617,8 @@
       <c r="E95" s="5"/>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
-      <c r="H95" s="7"/>
-    </row>
-    <row r="96" spans="1:8" ht="15">
+    </row>
+    <row r="96" spans="1:7" ht="15">
       <c r="A96" s="5" t="s">
         <v>92</v>
       </c>
@@ -2592,9 +2628,8 @@
       <c r="E96" s="5"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
-    </row>
-    <row r="97" spans="1:8" ht="15">
+    </row>
+    <row r="97" spans="1:7" ht="15">
       <c r="A97" s="5" t="s">
         <v>93</v>
       </c>
@@ -2604,9 +2639,8 @@
       <c r="E97" s="5"/>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
-      <c r="H97" s="7"/>
-    </row>
-    <row r="98" spans="1:8" ht="15">
+    </row>
+    <row r="98" spans="1:7" ht="15">
       <c r="A98" s="5" t="s">
         <v>94</v>
       </c>
@@ -2616,9 +2650,8 @@
       <c r="E98" s="5"/>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
-    </row>
-    <row r="99" spans="1:8" ht="15">
+    </row>
+    <row r="99" spans="1:7" ht="15">
       <c r="A99" s="5" t="s">
         <v>95</v>
       </c>
@@ -2628,11 +2661,10 @@
       <c r="E99" s="5"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
-    </row>
-    <row r="100" spans="1:8" ht="15">
+    </row>
+    <row r="100" spans="1:7" ht="15">
       <c r="A100" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="5"/>
@@ -2640,11 +2672,10 @@
       <c r="E100" s="5"/>
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
-      <c r="H100" s="7"/>
-    </row>
-    <row r="101" spans="1:8" ht="15">
+    </row>
+    <row r="101" spans="1:7" ht="15">
       <c r="A101" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2655,4 +2686,39 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479316B9-5F26-4845-8586-CB47362E2B3D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15">
+      <c r="A1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Day40 [LeetCode-#1154] Day of the Year
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF41D80-9FEE-429D-ADC7-CF0814FA68CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B10397-5B83-4DCE-94A5-1D196E4C2C0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -620,6 +620,10 @@
     <t>Design a stack that supports push, pop, top, and retrieving the minimum element in constant time.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Return the day number of the year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -627,7 +631,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -738,7 +742,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1213,10 +1217,10 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K46" sqref="K46"/>
+      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2017,10 +2021,18 @@
       <c r="A41" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+      <c r="B41" s="6">
+        <v>44193</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
     </row>

</xml_diff>

<commit_message>
Day41 [LeetCode-#118] Pascal's Triangle
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4530A2B6-16ED-402A-AB5A-7104972FA6E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D4B67D-6DFF-42C7-8ECE-045A67DCE96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -632,6 +632,31 @@
   <si>
     <t>* Convert string to DateTime
 * Calculate the day of the year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Output the first </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>numRows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> of Pascal's triangle.</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1226,11 +1251,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F36" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1242,7 +1267,7 @@
     <col min="5" max="5" width="90.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1822,8 +1847,8 @@
         <v>119</v>
       </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="1">
-        <v>1</v>
+      <c r="H31" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30">
@@ -1916,6 +1941,9 @@
       <c r="G35" s="8" t="s">
         <v>115</v>
       </c>
+      <c r="H35" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="185.25">
       <c r="A36" s="5" t="s">
@@ -1935,8 +1963,8 @@
       <c r="G36" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H36" s="1">
-        <v>15</v>
+      <c r="H36" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="85.5">
@@ -2049,15 +2077,26 @@
       <c r="G41" s="9" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="15">
+      <c r="H41" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="16.5">
       <c r="A42" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="B42" s="6">
+        <v>44194</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
     </row>

</xml_diff>

<commit_message>
Day42 ASP.NET Core MVC Shooping Cart (1)
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D4B67D-6DFF-42C7-8ECE-045A67DCE96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B5895B-04F0-402E-BDDF-5DA796559299}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="140">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -657,6 +657,10 @@
       </rPr>
       <t> of Pascal's triangle.</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a Shopping Cart  with ASP.NET Core MVC </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1252,10 +1256,10 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomRight" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2104,10 +2108,16 @@
       <c r="A43" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5"/>
+      <c r="B43" s="6">
+        <v>44195</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+      <c r="E43" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
     </row>

</xml_diff>

<commit_message>
Day43 ASP.NET Core MVC Shooping Cart (2)
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B5895B-04F0-402E-BDDF-5DA796559299}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985A6AEF-45A5-4830-8CF3-C3034C83F658}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="143">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -597,22 +597,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>所花費時間</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>(hr)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Stack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -661,6 +645,81 @@
   </si>
   <si>
     <t xml:space="preserve">Create a Shopping Cart  with ASP.NET Core MVC </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Create an ASP.NET Core MVC project
+2. Delete HomeController.cs in the Controllers folder and Home in the Views folder
+3. Create ProductController  under the Controllers folder
+4. Create a product class
+5. Update a product class
+  &gt; public string Id {get; set;}
+  &gt; public string Name {get; set;}
+  &gt; public string Price {get; set;}
+  &gt; public string Photo {get; set;}
+6. Create an item class
+  &gt; public Product Product{get; set;}
+  &gt; public int Quantity{get; set;}
+7. Add ViewModels folder
+8. Create ProductModel class
+9. Update ProductModel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>所花費時間</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>(半個小時為一個單位)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. Update ProductModel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>public List&lt;Product&gt; _products { get; set; }
+        public List&lt;Product&gt; findall()
+        {
+            _products = new List&lt;Product&gt;
+            {
+                new Product()
+                {
+                    Id = "1", Name = "flower1", Photo = "thumb1.jpg", Price = 2.80
+                },
+                new Product()
+                {
+                    Id = "2", Name = "flower2", Photo = "thumb2.jpg", Price = 3.50
+                },
+                new Product()
+                {
+                    Id = "3", Name = "flower3", Photo = "thumb3.jpg", Price = 4.45
+                },
+                new Product()
+                {
+                    Id = "4", Name = "flower4", Photo = "thumb4.jpg", Price = 3.70
+                },
+                new Product()
+                {
+                    Id = "5", Name = "flower5", Photo = "thumb5.jpg", Price = 5.00
+                }
+            };
+            return _products;
+        }
+        public Product find(string id)
+        {
+            List&lt;Product&gt; products = findall();
+            var prod = products.Where(a =&gt; a.Id == id).FirstOrDefault();
+            return prod;
+        }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -973,7 +1032,7 @@
     <tableColumn id="8" xr3:uid="{31DC304D-1D42-4DAF-B0CC-BDF494F91A9F}" name="Purpose" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{8148EAA2-148F-4A8C-92EC-EB9EE7D7668D}" name="Skill" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{04FB5744-EEEA-494D-902D-6F2FC2E61962}" name="Step by Step" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{F9A548FB-04A0-4F7C-AEDA-6DA3F2B4B3EE}" name="所花費時間(hr)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{F9A548FB-04A0-4F7C-AEDA-6DA3F2B4B3EE}" name="所花費時間(半個小時為一個單位)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1255,11 +1314,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E45" sqref="E45"/>
+      <selection pane="bottomRight" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1270,8 +1329,8 @@
     <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="90.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.125" customWidth="1"/>
+    <col min="8" max="8" width="35.125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1298,7 +1357,7 @@
         <v>98</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15">
@@ -1992,7 +2051,7 @@
         <v>125</v>
       </c>
       <c r="H37" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15">
@@ -2033,7 +2092,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16.5">
@@ -2047,15 +2106,15 @@
         <v>103</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>134</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
       <c r="H40" s="1">
-        <v>0.63</v>
+        <v>1.125</v>
       </c>
       <c r="K40" s="12"/>
     </row>
@@ -2073,16 +2132,16 @@
         <v>128</v>
       </c>
       <c r="E41" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G41" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F41" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>136</v>
-      </c>
       <c r="H41" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="16.5">
@@ -2099,12 +2158,12 @@
         <v>102</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:11" ht="15">
+    <row r="43" spans="1:11" ht="285">
       <c r="A43" s="5" t="s">
         <v>39</v>
       </c>
@@ -2116,23 +2175,36 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
+      <c r="H43" s="1">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="44" spans="1:11" ht="15">
       <c r="A44" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="5"/>
+      <c r="B44" s="6">
+        <v>44196</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="E44" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-    </row>
-    <row r="45" spans="1:11" ht="15">
+      <c r="G44" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="409.5">
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
@@ -2141,7 +2213,9 @@
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
+      <c r="G45" s="9" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="46" spans="1:11" ht="15">
       <c r="A46" s="5" t="s">

</xml_diff>

<commit_message>
Day44 ASP.NET Core MVC Shopping Cart (3)
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A28A53A-F62B-4AEF-95AC-E40C001B7355}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FC83A6-AA6F-4DCC-BD65-8E2E0345BD65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="142">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -682,11 +682,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9. Update ProductModel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>public List&lt;Product&gt; _products { get; set; }
+    <t>9. Update ProductModel
+public List&lt;Product&gt; _products { get; set; }
         public List&lt;Product&gt; findall()
         {
             _products = new List&lt;Product&gt;
@@ -1325,11 +1322,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F44" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H46" sqref="H46"/>
+      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2196,7 +2193,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15">
+    <row r="44" spans="1:11" ht="409.5">
       <c r="A44" s="5" t="s">
         <v>40</v>
       </c>
@@ -2211,25 +2208,27 @@
         <v>138</v>
       </c>
       <c r="F44" s="7"/>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="9" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="409.5">
+      <c r="H44" s="13">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15">
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="E45" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="F45" s="7"/>
-      <c r="G45" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="H45" s="13">
-        <v>0.875</v>
-      </c>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:11" ht="15">
       <c r="A46" s="5" t="s">

</xml_diff>

<commit_message>
Day45 ASP.NET Core MVC Shopping Cart (4)
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FC83A6-AA6F-4DCC-BD65-8E2E0345BD65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECFBF19-3521-4F80-B376-CF7F54B39D8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1323,7 +1323,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
@@ -2229,6 +2229,9 @@
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
+      <c r="H45" s="1">
+        <v>1.875</v>
+      </c>
     </row>
     <row r="46" spans="1:11" ht="15">
       <c r="A46" s="5" t="s">

</xml_diff>

<commit_message>
Day46 ASP.NET Core MVC Shopping Cart (5)
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECFBF19-3521-4F80-B376-CF7F54B39D8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D95198-F7FE-4091-BA42-8AE5F6DEEDC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="1485" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B004CB31-48D6-4DC8-BE15-69254DA30E88}</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B004CB31-48D6-4DC8-BE15-69254DA30E88}">
+      <text>
+        <t>[對話串註解]
+您的 Excel 版本可讓您讀取此對話串註解; 但若以較新的 Excel 版本開啟此檔案，將會移除對它進行的所有編輯。深入了解: https://go.microsoft.com/fwlink/?linkid=870924。
+註解:
+    不用寫程式碼細節</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="144">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -682,41 +700,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9. Update ProductModel
-public List&lt;Product&gt; _products { get; set; }
-        public List&lt;Product&gt; findall()
-        {
-            _products = new List&lt;Product&gt;
-            {
-                new Product()
-                {
-                    Id = "1", Name = "flower1", Photo = "thumb1.jpg", Price = 2.80
-                },
-                new Product()
-                {
-                    Id = "2", Name = "flower2", Photo = "thumb2.jpg", Price = 3.50
-                },
-                new Product()
-                {
-                    Id = "3", Name = "flower3", Photo = "thumb3.jpg", Price = 4.45
-                },
-                new Product()
-                {
-                    Id = "4", Name = "flower4", Photo = "thumb4.jpg", Price = 3.70
-                },
-                new Product()
-                {
-                    Id = "5", Name = "flower5", Photo = "thumb5.jpg", Price = 5.00
-                }
-            };
-            return _products;
-        }
-        public Product find(string id)
-        {
-            List&lt;Product&gt; products = findall();
-            var prod = products.Where(a =&gt; a.Id == id).FirstOrDefault();
-            return prod;
-        }</t>
+    <t xml:space="preserve">9. Update ProductModel
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. Delete Error.cshtml
+11. Add images into images folder
+12. Update ProductController
+13. Add Empty Razor View Index.cshtml
+14. Update Index.html
+15. Create a Product folder in Views
+16. Move Index.cshtml to Product
+17. Update Startup.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18. Add a new controller "Cartcontroller"
+19. Add a new folder "Helper"
+20. Add a new class "SessionHelper"
+21. Install Nuget "Newtonsoft.Json"
+21. Update SessionHelper</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -728,7 +732,7 @@
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -792,6 +796,12 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1027,6 +1037,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="WillardKang 康哲維" id="{8A68C93D-A513-4291-A8E8-1FD94A25C011}" userId="S::willard_kang@grobest.com::414bdbdc-8e2e-46b3-b454-0962d89ab7c5" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1318,15 +1334,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G1" dT="2021-01-02T23:43:36.12" personId="{8A68C93D-A513-4291-A8E8-1FD94A25C011}" id="{B004CB31-48D6-4DC8-BE15-69254DA30E88}">
+    <text>不用寫程式碼細節</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
+      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2193,7 +2217,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="409.5">
+    <row r="44" spans="1:11" ht="30">
       <c r="A44" s="5" t="s">
         <v>40</v>
       </c>
@@ -2215,11 +2239,13 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15">
+    <row r="45" spans="1:11" ht="114">
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="6">
+        <v>44197</v>
+      </c>
       <c r="C45" s="5" t="s">
         <v>100</v>
       </c>
@@ -2228,21 +2254,34 @@
         <v>138</v>
       </c>
       <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
+      <c r="G45" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="H45" s="1">
         <v>1.875</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15">
+    <row r="46" spans="1:11" ht="71.25">
       <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
+      <c r="B46" s="6">
+        <v>44198</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
+      <c r="G46" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="47" spans="1:11" ht="15">
       <c r="A47" s="5" t="s">
@@ -2847,8 +2886,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Day47 [LeetCode-#252] Meeting Rooms
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D95198-F7FE-4091-BA42-8AE5F6DEEDC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5F51D7-B369-48F6-8686-0BAC131B683E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4605" yWindow="1485" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="145">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -723,6 +723,10 @@
 21. Update SessionHelper</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Determine if a person could attend all meetings.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -732,7 +736,7 @@
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -796,12 +800,6 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1347,10 +1345,10 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2287,10 +2285,16 @@
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="5"/>
+      <c r="B47" s="6">
+        <v>44199</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
     </row>
@@ -2298,10 +2302,16 @@
       <c r="A48" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5"/>
+      <c r="B48" s="6">
+        <v>44200</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+      <c r="E48" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
     </row>

</xml_diff>

<commit_message>
Day48 [LeetCode-#1002] Find Common Characters
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5F51D7-B369-48F6-8686-0BAC131B683E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ECB194-A67E-4EC6-9948-F3EC9001558E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="144">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -407,10 +407,6 @@
       </rPr>
       <t>x1,y1,x2,y2,...,xn,yn]</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>未統計</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -684,22 +680,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>所花費時間</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>(半個小時為一個單位)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">9. Update ProductModel
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -725,6 +705,10 @@
   </si>
   <si>
     <t>Determine if a person could attend all meetings.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find the duplicate character in string array.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -736,7 +720,7 @@
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,14 +777,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -822,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -854,14 +830,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="13">
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -889,9 +862,6 @@
         <charset val="136"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1044,17 +1014,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{810993BB-277E-4BBC-8D8A-6CC291D7C060}" name="表格1" displayName="表格1" ref="A1:H101" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:H101" xr:uid="{9C8C2E40-E16F-435F-9A43-053065E55DB4}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{99B64B0C-7B02-42F0-9370-CE94A9D8F63E}" name="天數" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6DB2B110-1A72-42DF-A8B1-B343A1A0C427}" name="日期" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{E2F17329-26C5-4449-AAAF-C99CB7FEDC95}" name="類型" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{C61EBE76-371E-4E92-9EC6-7A0DCD08BB8F}" name="Topic" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{31DC304D-1D42-4DAF-B0CC-BDF494F91A9F}" name="Purpose" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{8148EAA2-148F-4A8C-92EC-EB9EE7D7668D}" name="Skill" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{04FB5744-EEEA-494D-902D-6F2FC2E61962}" name="Step by Step" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{F9A548FB-04A0-4F7C-AEDA-6DA3F2B4B3EE}" name="所花費時間(半個小時為一個單位)" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{810993BB-277E-4BBC-8D8A-6CC291D7C060}" name="表格1" displayName="表格1" ref="A1:G101" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:G101" xr:uid="{9C8C2E40-E16F-435F-9A43-053065E55DB4}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{99B64B0C-7B02-42F0-9370-CE94A9D8F63E}" name="天數" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{6DB2B110-1A72-42DF-A8B1-B343A1A0C427}" name="日期" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{E2F17329-26C5-4449-AAAF-C99CB7FEDC95}" name="類型" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{C61EBE76-371E-4E92-9EC6-7A0DCD08BB8F}" name="Topic" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{31DC304D-1D42-4DAF-B0CC-BDF494F91A9F}" name="Purpose" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{8148EAA2-148F-4A8C-92EC-EB9EE7D7668D}" name="Skill" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{04FB5744-EEEA-494D-902D-6F2FC2E61962}" name="Step by Step" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1342,13 +1311,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1357,14 +1326,13 @@
     <col min="2" max="2" width="12.5" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="90.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="90.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="68.125" customWidth="1"/>
-    <col min="8" max="8" width="35.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1386,11 +1354,8 @@
       <c r="G1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15">
+    </row>
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1404,11 +1369,8 @@
       <c r="E2" s="5"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+    </row>
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1422,11 +1384,8 @@
       <c r="E3" s="5"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15">
+    </row>
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1440,11 +1399,8 @@
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15">
+    </row>
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1458,11 +1414,8 @@
       <c r="E5" s="5"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15">
+    </row>
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1476,11 +1429,8 @@
       <c r="E6" s="5"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15">
+    </row>
+    <row r="7" spans="1:7" ht="15">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1494,11 +1444,8 @@
       <c r="E7" s="5"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15">
+    </row>
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1512,11 +1459,8 @@
       <c r="E8" s="5"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15">
+    </row>
+    <row r="9" spans="1:7" ht="15">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1530,11 +1474,8 @@
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15">
+    </row>
+    <row r="10" spans="1:7" ht="15">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -1548,11 +1489,8 @@
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15">
+    </row>
+    <row r="11" spans="1:7" ht="15">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1566,11 +1504,8 @@
       <c r="E11" s="5"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15">
+    </row>
+    <row r="12" spans="1:7" ht="15">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1584,11 +1519,8 @@
       <c r="E12" s="5"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15">
+    </row>
+    <row r="13" spans="1:7" ht="15">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1602,11 +1534,8 @@
       <c r="E13" s="5"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15">
+    </row>
+    <row r="14" spans="1:7" ht="15">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -1620,11 +1549,8 @@
       <c r="E14" s="5"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15">
+    </row>
+    <row r="15" spans="1:7" ht="15">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1638,11 +1564,8 @@
       <c r="E15" s="5"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15">
+    </row>
+    <row r="16" spans="1:7" ht="15">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -1656,11 +1579,8 @@
       <c r="E16" s="5"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15">
+    </row>
+    <row r="17" spans="1:7" ht="15">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
@@ -1674,11 +1594,8 @@
       <c r="E17" s="5"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15">
+    </row>
+    <row r="18" spans="1:7" ht="15">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1692,11 +1609,8 @@
       <c r="E18" s="5"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15">
+    </row>
+    <row r="19" spans="1:7" ht="15">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1710,11 +1624,8 @@
       <c r="E19" s="5"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15">
+    </row>
+    <row r="20" spans="1:7" ht="15">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -1728,11 +1639,8 @@
       <c r="E20" s="5"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15">
+    </row>
+    <row r="21" spans="1:7" ht="15">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1746,11 +1654,8 @@
       <c r="E21" s="5"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15">
+    </row>
+    <row r="22" spans="1:7" ht="15">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1764,11 +1669,8 @@
       <c r="E22" s="5"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15">
+    </row>
+    <row r="23" spans="1:7" ht="15">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1782,11 +1684,8 @@
       <c r="E23" s="5"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15">
+    </row>
+    <row r="24" spans="1:7" ht="15">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1800,11 +1699,8 @@
       <c r="E24" s="5"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15">
+    </row>
+    <row r="25" spans="1:7" ht="15">
       <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1818,11 +1714,8 @@
       <c r="E25" s="5"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15">
+    </row>
+    <row r="26" spans="1:7" ht="15">
       <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
@@ -1836,11 +1729,8 @@
       <c r="E26" s="5"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15">
+    </row>
+    <row r="27" spans="1:7" ht="15">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
@@ -1854,11 +1744,8 @@
       <c r="E27" s="5"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15">
+    </row>
+    <row r="28" spans="1:7" ht="15">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
@@ -1872,11 +1759,8 @@
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15">
+    </row>
+    <row r="29" spans="1:7" ht="15">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
@@ -1892,11 +1776,8 @@
       <c r="E29" s="5"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="45">
+    </row>
+    <row r="30" spans="1:7" ht="45">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
@@ -1910,17 +1791,14 @@
         <v>102</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="16.5">
+    </row>
+    <row r="31" spans="1:7" ht="16.5">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -1934,17 +1812,14 @@
         <v>102</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30">
+    </row>
+    <row r="32" spans="1:7" ht="30">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
@@ -1961,14 +1836,11 @@
         <v>108</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="30">
+    </row>
+    <row r="33" spans="1:10" ht="30">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -1985,18 +1857,15 @@
         <v>107</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="57">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="57">
       <c r="A34" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="6">
         <v>44186</v>
@@ -2012,13 +1881,10 @@
       <c r="G34" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="261" customHeight="1">
+    </row>
+    <row r="35" spans="1:10" ht="261" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B35" s="6">
         <v>44187</v>
@@ -2028,19 +1894,16 @@
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="185.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="185.25">
       <c r="A36" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="6">
         <v>44188</v>
@@ -2050,17 +1913,14 @@
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="71.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="71.25">
       <c r="A37" s="5" t="s">
         <v>33</v>
       </c>
@@ -2071,20 +1931,17 @@
         <v>103</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15">
       <c r="A38" s="5" t="s">
         <v>34</v>
       </c>
@@ -2095,15 +1952,15 @@
         <v>103</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:11" ht="16.5">
+    <row r="39" spans="1:10" ht="16.5">
       <c r="A39" s="5" t="s">
         <v>35</v>
       </c>
@@ -2114,18 +1971,15 @@
         <v>103</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
-      <c r="H39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="16.5">
+    </row>
+    <row r="40" spans="1:10" ht="16.5">
       <c r="A40" s="5" t="s">
         <v>36</v>
       </c>
@@ -2136,19 +1990,16 @@
         <v>103</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="1">
-        <v>1.125</v>
-      </c>
-      <c r="K40" s="12"/>
-    </row>
-    <row r="41" spans="1:11" ht="30">
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="1:10" ht="30">
       <c r="A41" s="5" t="s">
         <v>37</v>
       </c>
@@ -2159,22 +2010,19 @@
         <v>103</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E41" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="F41" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="16.5">
+    </row>
+    <row r="42" spans="1:10" ht="16.5">
       <c r="A42" s="5" t="s">
         <v>38</v>
       </c>
@@ -2188,12 +2036,12 @@
         <v>102</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:11" ht="242.25">
+    <row r="43" spans="1:10" ht="242.25">
       <c r="A43" s="5" t="s">
         <v>39</v>
       </c>
@@ -2205,17 +2053,14 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="H43" s="1">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="30">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="30">
       <c r="A44" s="5" t="s">
         <v>40</v>
       </c>
@@ -2227,17 +2072,14 @@
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H44" s="13">
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="114">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="114">
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
@@ -2249,17 +2091,14 @@
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="H45" s="1">
-        <v>1.875</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="71.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="71.25">
       <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
@@ -2271,17 +2110,14 @@
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="H46" s="1">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15">
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
@@ -2293,12 +2129,12 @@
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:11" ht="15">
+    <row r="48" spans="1:10" ht="15">
       <c r="A48" s="5" t="s">
         <v>44</v>
       </c>
@@ -2310,7 +2146,7 @@
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
@@ -2319,10 +2155,16 @@
       <c r="A49" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="5"/>
+      <c r="B49" s="6">
+        <v>44201</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
     </row>
@@ -2878,7 +2720,7 @@
     </row>
     <row r="100" spans="1:7" ht="15">
       <c r="A100" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="5"/>
@@ -2889,7 +2731,7 @@
     </row>
     <row r="101" spans="1:7" ht="15">
       <c r="A101" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2922,7 +2764,7 @@
         <v>105</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Day49 [LeetCode-#1122] Relative Sort ArrayRelativeSortArray
</commit_message>
<xml_diff>
--- a/100Days_C#.xlsx
+++ b/100Days_C#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\C#\myProject\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B0F2E2-4814-4982-BC49-C467447DE0D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68A0BE4-2EFC-418F-B080-1700FB90FA78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="統計" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="144">
   <si>
     <t>天數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -836,15 +836,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <font>
-        <name val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -875,6 +866,15 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1028,19 +1028,19 @@
     <tableColumn id="3" xr3:uid="{E2F17329-26C5-4449-AAAF-C99CB7FEDC95}" name="類型" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{C61EBE76-371E-4E92-9EC6-7A0DCD08BB8F}" name="Topic" dataDxfId="7"/>
     <tableColumn id="8" xr3:uid="{31DC304D-1D42-4DAF-B0CC-BDF494F91A9F}" name="Purpose" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{04FB5744-EEEA-494D-902D-6F2FC2E61962}" name="Step by Step" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{8148EAA2-148F-4A8C-92EC-EB9EE7D7668D}" name="Skill" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{04FB5744-EEEA-494D-902D-6F2FC2E61962}" name="Step by Step" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8148EAA2-148F-4A8C-92EC-EB9EE7D7668D}" name="Skill" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AABD3024-27F9-4340-9F92-F8142ABB2B4D}" name="表格2" displayName="表格2" ref="A1:B2" insertRow="1" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AABD3024-27F9-4340-9F92-F8142ABB2B4D}" name="表格2" displayName="表格2" ref="A1:B2" insertRow="1" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B2" xr:uid="{319BFF1A-00BE-462B-A13D-51F0FB7E00A8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3C41B99C-6466-4DFC-B371-702A032EAC39}" name="Skill" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{EF89176C-D56C-42F7-B7FE-8446C1093E92}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3C41B99C-6466-4DFC-B371-702A032EAC39}" name="Skill" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{EF89176C-D56C-42F7-B7FE-8446C1093E92}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1320,10 +1320,10 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E56" sqref="E56"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2178,8 +2178,12 @@
       <c r="A50" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="5"/>
+      <c r="B50" s="6">
+        <v>44202</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="7"/>

</xml_diff>